<commit_message>
Aluminum parts, material change to 6061 Aluminum
Revised CHECON.FACE and CHECON.BACK drawings to v1.1 rev B
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Release ID</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>Found that thicker CHECON.COVER better protected screen</t>
+  </si>
+  <si>
+    <t>CHECON.MECH.v1.2</t>
+  </si>
+  <si>
+    <t>Material changed to 6061 Aluminum</t>
+  </si>
+  <si>
+    <t>Materials change initiated by supplier, improvement to anodizing</t>
   </si>
 </sst>
 </file>
@@ -74,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -82,11 +91,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -153,19 +157,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -189,92 +193,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1262047</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Shape 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="-266700"/>
-          <a:ext cx="2684448" cy="365126"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" marL="0" marR="0" indent="0" algn="l" defTabSz="457200">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1400" u="none">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:sym typeface="Helvetica"/>
-            </a:rPr>
-            <a:t>CHECON.MECH.ECO</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1503,69 +1421,105 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L14"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="43.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="1" customWidth="1"/>
-    <col min="13" max="256" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="1" customWidth="1"/>
+    <col min="12" max="256" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.95" customHeight="1"/>
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
+    </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="B2" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s" s="2">
-        <v>10</v>
+      <c r="A2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4">
+        <v>42100</v>
       </c>
     </row>
-    <row r="3" ht="31" customHeight="1">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="s" s="3">
+        <v>15</v>
+      </c>
       <c r="B3" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="3">
         <v>12</v>
@@ -1583,54 +1537,40 @@
         <v>12</v>
       </c>
       <c r="I3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4">
+        <v>42101</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="K3" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="L3" s="4">
-        <v>42100</v>
-      </c>
-    </row>
-    <row r="4" ht="44" customHeight="1">
-      <c r="B4" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s" s="3">
-        <v>12</v>
-      </c>
       <c r="J4" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="L4" s="4">
-        <v>42101</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1641,9 +1581,9 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1654,9 +1594,9 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1667,9 +1607,9 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1680,9 +1620,9 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
+      <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1693,9 +1633,9 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
+      <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1706,9 +1646,9 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1719,9 +1659,9 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1732,9 +1672,9 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1745,20 +1685,6 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1766,7 +1692,5 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added line for latests update
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Release ID</t>
   </si>
   <si>
+    <t>MISC Change</t>
+  </si>
+  <si>
     <t>FACE Change</t>
   </si>
   <si>
@@ -74,14 +77,24 @@
   </si>
   <si>
     <t>Materials change initiated by supplier, improvement to anodizing</t>
+  </si>
+  <si>
+    <t>CHECON.MECH.v.1.3</t>
+  </si>
+  <si>
+    <t>Added BOM</t>
+  </si>
+  <si>
+    <t>Subassembly requires its own BOM (value add)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -95,14 +108,14 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <b val="1"/>
@@ -153,12 +166,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -166,10 +179,16 @@
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1421,7 +1440,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1430,15 +1449,16 @@
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.375" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.25" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="1" customWidth="1"/>
-    <col min="12" max="256" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="43.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="1" customWidth="1"/>
+    <col min="13" max="256" width="13" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
@@ -1475,31 +1495,32 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s" s="3">
         <v>12</v>
       </c>
+      <c r="B2" s="4"/>
       <c r="C2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s" s="3">
         <v>13</v>
@@ -1507,184 +1528,224 @@
       <c r="J2" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5">
         <v>42100</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s" s="3">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3" t="s" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s" s="3">
         <v>13</v>
       </c>
       <c r="J3" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="L3" s="5">
         <v>42101</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" t="s" s="3">
-        <v>19</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" t="s" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="K4" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="K4" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="L4" s="7">
+        <v>42116</v>
+      </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="A5" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="L5" s="7">
+        <v>42129</v>
+      </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Initial commit, CHECON.MECH v1.4
Took out a part, added a new one. Edits & updates to .MECH.BOM and
.MECH.ECO
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Release ID</t>
   </si>
@@ -29,6 +29,9 @@
     <t>COVER Change</t>
   </si>
   <si>
+    <t>CLIP Change</t>
+  </si>
+  <si>
     <t>TRAY Change</t>
   </si>
   <si>
@@ -90,17 +93,105 @@
   </si>
   <si>
     <t>Subassembly requires its own BOM (value add)</t>
+  </si>
+  <si>
+    <t>CHECON.MECH.v.1.4</t>
+  </si>
+  <si>
+    <r>
+      <t>Added 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> CHECON.CORETOP, Deleted CHECON.TRAY,</t>
+    </r>
+  </si>
+  <si>
+    <t>Introduced new part</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <r>
+      <t>Added 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> CORETOP, deleted slots that CHECON.TRAY rested in</t>
+    </r>
+  </si>
+  <si>
+    <t>Removed 0.9mm drop for PCB, shrunk the antenna slot </t>
+  </si>
+  <si>
+    <t>Shrunk the antenna slot</t>
+  </si>
+  <si>
+    <r>
+      <t>Added screen backlight. Necessitated the addition of a 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> CORETOP part, and resulted in the removal of several machining operations from core parts.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -123,6 +214,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -130,6 +227,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,12 +242,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -185,29 +290,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -227,21 +336,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="1" width="14"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="1" width="9.37407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.2518518518519"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="43.2555555555556"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.0037037037037"/>
-    <col collapsed="false" hidden="false" max="256" min="13" style="1" width="13"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="2" width="13"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.37407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.6740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.8888888888889"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.2518518518519"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="43.2555555555556"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.0037037037037"/>
+    <col collapsed="false" hidden="false" max="257" min="14" style="1" width="13"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="2" width="13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -281,32 +394,33 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>14</v>
@@ -314,118 +428,165 @@
       <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="n">
         <v>42100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="5" t="n">
         <v>42101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="5" t="n">
         <v>42116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5" t="n">
         <v>42129</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="6" t="n">
+        <v>42201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHECON v1.1 initial commit production files
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -592,7 +592,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>

</xml_diff>

<commit_message>
Correction to ECO of copied messages
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -221,7 +221,7 @@
     </r>
   </si>
   <si>
-    <t>CHECON.MECH initial file commit</t>
+    <t>CHECON.MECH Derivative file commit</t>
   </si>
   <si>
     <t>CHECON.MECH V1.1 initial commit production files</t>
@@ -248,7 +248,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -271,12 +271,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -290,11 +284,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -304,6 +293,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -369,35 +364,35 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,10 +413,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -841,76 +836,77 @@
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="7" t="s">
+      <c r="K17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="8" t="n">
+      <c r="N17" s="7" t="n">
         <v>42201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>

</xml_diff>

<commit_message>
Updates to ECO for v1.5
</commit_message>
<xml_diff>
--- a/CHECON.MECH.ECO.xlsx
+++ b/CHECON.MECH.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>Release ID</t>
   </si>
@@ -237,6 +237,36 @@
   </si>
   <si>
     <t>Updated lasercut readme files to new format</t>
+  </si>
+  <si>
+    <t>Edits to CHECON.MECH.ECO (copied commit messages) and CHECON.MECH.BOM (release tag and minor edit)</t>
+  </si>
+  <si>
+    <t>Correction to ECO of copied messages</t>
+  </si>
+  <si>
+    <t>Final edit to BOM - date correction</t>
+  </si>
+  <si>
+    <t>CHECON.MECH v1.5: Copied CHECON.TRAY v1.0 REV A and CHECON.CORETOP v1.0 REV A folders back into directory, deleted CHECON.CLIP v1.0 REV A folder</t>
+  </si>
+  <si>
+    <t>File name updates for clarity</t>
+  </si>
+  <si>
+    <t>CHECON.MECH.v.1.5</t>
+  </si>
+  <si>
+    <t>Temporarily deleted. Will come back in v1.6</t>
+  </si>
+  <si>
+    <t>Reverted to VER 1.0 REV A</t>
+  </si>
+  <si>
+    <t>As above for v1.4</t>
+  </si>
+  <si>
+    <t>Production needs necessitated forking dev paths for the Happy Antenna and Backlight versions of the CHECON. Some parts reverted to previous versions (as noted) and others modified (as noted). </t>
   </si>
 </sst>
 </file>
@@ -271,13 +301,13 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -298,7 +328,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Verdana"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -311,7 +342,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -324,13 +355,6 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -359,40 +383,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,17 +433,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="14"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.9481481481482"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.37407407407407"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8444444444444"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.6740740740741"/>
@@ -832,81 +855,143 @@
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="68.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="54.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="6" t="s">
+      <c r="K17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="7" t="n">
+      <c r="N17" s="6" t="n">
         <v>42201</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8" t="s">
+    <row r="18" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8" t="s">
+    <row r="19" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+    <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8" t="s">
+    <row r="21" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="8" t="s">
+    <row r="23" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="58.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="6" t="n">
+        <v>42219</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>

</xml_diff>